<commit_message>
Added README file and an example for time calculation file
</commit_message>
<xml_diff>
--- a/Time from the given event.xlsx
+++ b/Time from the given event.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/10ea117026847637/Pulpit/Portfolio/Excel or Google Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/10ea117026847637/GitHub/Excel-or-Google-Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="564" documentId="14_{3841E665-0981-4D29-939B-3D5544C82E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{916A6563-816A-45EA-B127-16E5B8798922}"/>
@@ -740,7 +740,7 @@
   <dimension ref="B1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,7 +806,7 @@
       </c>
       <c r="D7" s="33">
         <f ca="1">IF($K$6=1, TODAY(), "Give the date below:")</f>
-        <v>45415</v>
+        <v>45424</v>
       </c>
       <c r="E7" s="34"/>
       <c r="F7" s="2"/>
@@ -848,7 +848,7 @@
       </c>
       <c r="C11" s="28" t="str">
         <f ca="1">IF(D4="","",IFERROR(IF($K$6=1,DATEDIF($D$4,TODAY(),"Y") &amp; " Years, " &amp; DATEDIF($D$4,TODAY(),"YM") &amp; " Months, " &amp; DATEDIF($D$4,TODAY(),"MD") &amp; " Days", IF(ISNUMBER($C$8), DATEDIF($D$4, $C$8,"Y") &amp; " Years, " &amp; DATEDIF($D$4, $C$8,"YM") &amp; " Months, " &amp; DATEDIF($D$4, $C$8,"MD") &amp; " Days", "")),""))</f>
-        <v>20 Years, 0 Months, 2 Days</v>
+        <v>20 Years, 0 Months, 11 Days</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="30"/>
@@ -870,7 +870,7 @@
       </c>
       <c r="C13" s="19">
         <f ca="1">IF(D4="","",IFERROR(IF($K$6=1,DATEDIF($D$4,TODAY(),"d"), IF(ISNUMBER($C$8),DATEDIF($D$4, $C$8,"d"), "")),""))</f>
-        <v>7307</v>
+        <v>7316</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>

</xml_diff>